<commit_message>
More updates to the MS and revision letter
</commit_message>
<xml_diff>
--- a/data/HOMA IR.xlsx
+++ b/data/HOMA IR.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
   <si>
     <t>Mouse</t>
   </si>
@@ -56,15 +56,6 @@
     <t>HOMA-IR</t>
   </si>
   <si>
-    <t>Insulin- pmol/L</t>
-  </si>
-  <si>
-    <t>Insulin- uIU/mL</t>
-  </si>
-  <si>
-    <t>Glucose- mmol/L</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
@@ -78,6 +69,24 @@
   </si>
   <si>
     <t>Ttest</t>
+  </si>
+  <si>
+    <t>Mouse 206 is excluded from analysis because it had malocclusion</t>
+  </si>
+  <si>
+    <t>Glucose-mmol/L</t>
+  </si>
+  <si>
+    <t>Insulin-pmol/L</t>
+  </si>
+  <si>
+    <t>Insulin-uIU/mL</t>
+  </si>
+  <si>
+    <t>Insulin pmol.L</t>
+  </si>
+  <si>
+    <t>Glucose mmol.L</t>
   </si>
 </sst>
 </file>
@@ -85,13 +94,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,10 +133,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,19 +422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
@@ -436,16 +458,16 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>202</v>
       </c>
@@ -463,7 +485,7 @@
         <v>10.166666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>201</v>
       </c>
@@ -480,8 +502,23 @@
         <f t="shared" ref="E3:E26" si="0">D3/18</f>
         <v>12.555555555555555</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="P3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="T3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>203</v>
       </c>
@@ -506,7 +543,7 @@
         <v>1.098317</v>
       </c>
       <c r="H4">
-        <f>G4*1000*1/5808*1000</f>
+        <f t="shared" ref="H4:H26" si="1">G4*1000*1/5808*1000</f>
         <v>189.10416666666666</v>
       </c>
       <c r="I4" s="1">
@@ -523,8 +560,20 @@
       <c r="N4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>204</v>
       </c>
@@ -545,23 +594,23 @@
         <v>963.89880000000005</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G26" si="1">(F5/1000)</f>
+        <f t="shared" ref="G5:G26" si="2">(F5/1000)</f>
         <v>0.96389880000000006</v>
       </c>
       <c r="H5">
-        <f>G5*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>165.96053719008268</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I26" si="2">H5/6</f>
+        <f t="shared" ref="I5:I26" si="3">H5/6</f>
         <v>27.660089531680445</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J26" si="3">(I5*D5)/405</f>
+        <f t="shared" ref="J5:J26" si="4">(I5*D5)/405</f>
         <v>9.0151402918069596</v>
       </c>
       <c r="L5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M5">
         <f>AVERAGE(J13:J26)</f>
@@ -571,8 +620,30 @@
         <f>AVERAGE(J4:J11)</f>
         <v>12.141325674321781</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <f>AVERAGE(H13:H26)</f>
+        <v>174.16515889413617</v>
+      </c>
+      <c r="R5">
+        <f>AVERAGE(H4:H11)</f>
+        <v>175.10476928374655</v>
+      </c>
+      <c r="T5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <f>AVERAGE(E13:E26)</f>
+        <v>9.7301587301587311</v>
+      </c>
+      <c r="V5">
+        <f>AVERAGE(E2:E11)</f>
+        <v>10.061111111111112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>207</v>
       </c>
@@ -593,23 +664,23 @@
         <v>1029.605</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0296050000000001</v>
       </c>
       <c r="H6">
-        <f>G6*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>177.27358815426996</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.545598025711659</v>
       </c>
       <c r="J6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.058424806425647</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M6">
         <f>STDEV(J13:J26)</f>
@@ -619,8 +690,30 @@
         <f>STDEV(J4:J11)</f>
         <v>2.7140065671365279</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <f>STDEV(H13:H26)</f>
+        <v>55.114744050733904</v>
+      </c>
+      <c r="R6">
+        <f>STDEV(H4:H11)</f>
+        <v>52.864977284266388</v>
+      </c>
+      <c r="T6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U6">
+        <f>STDEV(E13:E26)</f>
+        <v>1.3315260441669672</v>
+      </c>
+      <c r="V6">
+        <f>STDEV(E2:E11)</f>
+        <v>2.1742428478877915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>208</v>
       </c>
@@ -641,23 +734,23 @@
         <v>922.27499999999998</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92227499999999996</v>
       </c>
       <c r="H7">
-        <f>G7*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>158.79390495867767</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26.465650826446279</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.566469620446892</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M7">
         <f>COUNT(J13:J26)</f>
@@ -667,8 +760,30 @@
         <f>COUNT(J4:J11)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7">
+        <f>COUNT(H13:H26)</f>
+        <v>14</v>
+      </c>
+      <c r="R7">
+        <f>COUNT(H4:H11)</f>
+        <v>8</v>
+      </c>
+      <c r="T7" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7">
+        <f>COUNT(E13:E26)</f>
+        <v>14</v>
+      </c>
+      <c r="V7">
+        <f>COUNT(E2:E11)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>209</v>
       </c>
@@ -689,23 +804,23 @@
         <v>573.7432</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.57374320000000001</v>
       </c>
       <c r="H8">
-        <f>G8*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>98.784986225895324</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.464164370982555</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.8865379949891743</v>
       </c>
       <c r="L8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M8">
         <f>M6/SQRT(M7)</f>
@@ -715,8 +830,30 @@
         <f>N6/SQRT(N7)</f>
         <v>0.95954622390353084</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8">
+        <f>Q6/SQRT(Q7)</f>
+        <v>14.730034942684547</v>
+      </c>
+      <c r="R8">
+        <f>R6/SQRT(R7)</f>
+        <v>18.690591962488778</v>
+      </c>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="U8">
+        <f>U6/SQRT(U7)</f>
+        <v>0.35586530420280132</v>
+      </c>
+      <c r="V8">
+        <f>V6/SQRT(V7)</f>
+        <v>0.68755595856564389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>214</v>
       </c>
@@ -737,30 +874,44 @@
         <v>1058.03</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.05803</v>
       </c>
       <c r="H9">
-        <f>G9*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>182.16769972451792</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30.361283287419653</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.844648788672357</v>
       </c>
       <c r="L9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M9">
         <f>TTEST(J13:J26,J4:J11,2,3)</f>
         <v>0.70254597760929749</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9">
+        <f>TTEST(H13:H26,H4:H11,2,3)</f>
+        <v>0.96901748241144403</v>
+      </c>
+      <c r="T9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9">
+        <f>TTEST(E13:E26,E2:E11,2,3)</f>
+        <v>0.67563212532208994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>250</v>
       </c>
@@ -781,23 +932,23 @@
         <v>1656.883</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6568830000000001</v>
       </c>
       <c r="H10">
-        <f>G10*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>285.2759986225895</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47.545999770431585</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.38331845389926</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2500</v>
       </c>
@@ -818,60 +969,63 @@
         <v>833.31600000000003</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83331600000000006</v>
       </c>
       <c r="H11">
-        <f>G11*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>143.47727272727272</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23.912878787878785</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.111550692106247</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>206</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
         <v>136</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <f>D12/18</f>
         <v>7.5555555555555554</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>452.99740000000003</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <f>(F12/1000)</f>
         <v>0.45299740000000005</v>
       </c>
-      <c r="H12">
-        <f>G12*1000*1/5808*1000</f>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
         <v>77.995420110192839</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="4">
         <f>H12/6</f>
         <v>12.999236685032139</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <f>(I12*D12)/405</f>
         <v>4.365175775714496</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>291</v>
       </c>
@@ -892,23 +1046,23 @@
         <v>1033.6780000000001</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0336780000000001</v>
       </c>
       <c r="H13">
-        <f>G13*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>177.97486225895318</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.662477043158862</v>
       </c>
       <c r="J13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.5212889274337087</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>294</v>
       </c>
@@ -929,23 +1083,23 @@
         <v>1561.885</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.561885</v>
       </c>
       <c r="H14">
-        <f>G14*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>268.91959366391183</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44.819932277318635</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21.690633892233215</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>298</v>
       </c>
@@ -966,23 +1120,23 @@
         <v>1130.288</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.130288</v>
       </c>
       <c r="H15">
-        <f>G15*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>194.60881542699724</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32.434802571166209</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.296413064426533</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>292</v>
       </c>
@@ -1003,19 +1157,19 @@
         <v>417.81619999999998</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.41781619999999997</v>
       </c>
       <c r="H16">
-        <f>G16*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>71.938050964187326</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.989675160697887</v>
       </c>
       <c r="J16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2925997488918366</v>
       </c>
     </row>
@@ -1040,19 +1194,19 @@
         <v>918.08780000000002</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.91808780000000001</v>
       </c>
       <c r="H17">
-        <f>G17*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>158.07296831955921</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26.345494719926535</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.441234142774544</v>
       </c>
     </row>
@@ -1077,19 +1231,19 @@
         <v>608.72670000000005</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60872670000000006</v>
       </c>
       <c r="H18">
-        <f>G18*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>104.80831611570248</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.468052685950415</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.2539941715131109</v>
       </c>
     </row>
@@ -1114,19 +1268,19 @@
         <v>892.86469999999997</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89286469999999996</v>
       </c>
       <c r="H19">
-        <f>G19*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>153.73014807162534</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25.621691345270889</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.703735552778062</v>
       </c>
     </row>
@@ -1151,19 +1305,19 @@
         <v>901.29139999999995</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90129139999999996</v>
       </c>
       <c r="H20">
-        <f>G20*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>155.1810261707989</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25.863504361799816</v>
       </c>
       <c r="J20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.345401744719926</v>
       </c>
     </row>
@@ -1188,19 +1342,19 @@
         <v>1304.3610000000001</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3043610000000001</v>
       </c>
       <c r="H21">
-        <f>G21*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>224.58006198347107</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.430010330578511</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.635560146923783</v>
       </c>
     </row>
@@ -1225,19 +1379,19 @@
         <v>934.80960000000005</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93480960000000002</v>
       </c>
       <c r="H22">
-        <f>G22*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>160.95206611570248</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26.82534435261708</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.193785668129102</v>
       </c>
     </row>
@@ -1262,19 +1416,19 @@
         <v>816.11350000000004</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81611350000000005</v>
       </c>
       <c r="H23">
-        <f>G23*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>140.51540977961432</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23.419234963269052</v>
       </c>
       <c r="J23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.639849958621001</v>
       </c>
     </row>
@@ -1299,19 +1453,19 @@
         <v>1181.778</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.181778</v>
       </c>
       <c r="H24">
-        <f>G24*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>203.47417355371903</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33.912362258953173</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.151084498180461</v>
       </c>
     </row>
@@ -1336,19 +1490,19 @@
         <v>1554.52</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5545199999999999</v>
       </c>
       <c r="H25">
-        <f>G25*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>267.65151515151513</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44.608585858585855</v>
       </c>
       <c r="J25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20.486906098017204</v>
       </c>
     </row>
@@ -1373,19 +1527,19 @@
         <v>905.49749999999995</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90549749999999996</v>
       </c>
       <c r="H26">
-        <f>G26*1000*1/5808*1000</f>
+        <f t="shared" si="1"/>
         <v>155.90521694214877</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25.984202823691462</v>
       </c>
       <c r="J26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.061802792232086</v>
       </c>
     </row>
@@ -1402,6 +1556,11 @@
       <c r="I35" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="T3:V3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>